<commit_message>
cambio en el login de la aplicacion
</commit_message>
<xml_diff>
--- a/registro_persona_natural.xlsx
+++ b/registro_persona_natural.xlsx
@@ -397,9 +397,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
@@ -430,9 +430,23 @@
         <v>1730178167639-reporte_estudiante (2).pdf</v>
       </c>
     </row>
+    <row r="3">
+      <c r="A3" t="str">
+        <v>Prueba</v>
+      </c>
+      <c r="B3" t="str">
+        <v>Bautista</v>
+      </c>
+      <c r="C3" t="str">
+        <v>jbautmqpea@gmail.com</v>
+      </c>
+      <c r="D3" t="str">
+        <v>1730224973880-ATS CV harvard (1).pdf</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D2"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
mandando correo a direccion establecida
</commit_message>
<xml_diff>
--- a/registro_persona_natural.xlsx
+++ b/registro_persona_natural.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
     <sheetView workbookViewId="0" rightToLeft="0"/>
   </sheetViews>
@@ -444,9 +444,233 @@
         <v>1730224973880-ATS CV harvard (1).pdf</v>
       </c>
     </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B4" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C4" t="str">
+        <v>sslsc@udistrital.edu.co</v>
+      </c>
+      <c r="D4" t="str">
+        <v>1730262733833-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B5" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C5" t="str">
+        <v>sslsc@udistrital.edu.co</v>
+      </c>
+      <c r="D5" t="str">
+        <v>1730262850260-Escudo_UD.png</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B6" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C6" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D6" t="str">
+        <v>1730262972598-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B7" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C7" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D7" t="str">
+        <v>1730263075607-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B8" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C8" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D8" t="str">
+        <v>1730263362238-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B9" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C9" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D9" t="str">
+        <v>1730263606699-Ejercicios ED HomogeÌneas.pdf</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B10" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C10" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D10" t="str">
+        <v>1730263744368-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B11" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C11" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D11" t="str">
+        <v>1730263775745-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B12" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C12" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D12" t="str">
+        <v>1730264179945-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B13" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C13" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D13" t="str">
+        <v>1730264270327-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B14" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C14" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D14" t="str">
+        <v>1730265483895-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B15" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C15" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D15" t="str">
+        <v>1730265556103-Ejercicios ED Exactas.pdf</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B16" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C16" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D16" t="str">
+        <v>1730265720556-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B17" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C17" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D17" t="str">
+        <v>1730265909314-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B18" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C18" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D18" t="str">
+        <v>1730266029793-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="str">
+        <v>Juan Pablo</v>
+      </c>
+      <c r="B19" t="str">
+        <v>Bautista Clavijo</v>
+      </c>
+      <c r="C19" t="str">
+        <v>jbautistaclavijo@gmail.com</v>
+      </c>
+      <c r="D19" t="str">
+        <v>1730266224051-reporte_estudiante (2).pdf</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D19"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>